<commit_message>
Assignment 5 - Complete
</commit_message>
<xml_diff>
--- a/Assignment5/Book1.xlsx
+++ b/Assignment5/Book1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="22995" windowHeight="11055"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="22995" windowHeight="11055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="21">
   <si>
     <t>A</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>SW3</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -87,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -97,6 +103,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -128,12 +140,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="18" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="A17:I20"/>
     </sheetView>
   </sheetViews>
@@ -1061,12 +1076,138 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="B2" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="B3" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="B4" s="7">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="D4">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>0.75</v>
+      </c>
+      <c r="B7">
+        <v>20</v>
+      </c>
+      <c r="C7">
+        <v>17.329999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="B8" s="7">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>22.33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="B9" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>0.875</v>
+      </c>
+      <c r="B10" s="7">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>26.67</v>
+      </c>
+      <c r="D10">
+        <v>26.67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="B11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="B12">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>30</v>
+      </c>
+      <c r="D12">
+        <v>27.33</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>